<commit_message>
feat: update course example spreadsheet
</commit_message>
<xml_diff>
--- a/examples/course_example.xlsx
+++ b/examples/course_example.xlsx
@@ -42,16 +42,10 @@
       <style:table-row-properties style:row-height="0.178in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro2" style:family="table-row">
+      <style:table-row-properties style:row-height="0.4866in" fo:break-before="auto" style:use-optimal-row-height="true"/>
+    </style:style>
+    <style:style style:name="ro3" style:family="table-row">
       <style:table-row-properties style:row-height="0.3311in" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="1.2638in" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro4" style:family="table-row">
-      <style:table-row-properties style:row-height="0.4866in" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro5" style:family="table-row">
-      <style:table-row-properties style:row-height="0.6425in" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -103,42 +97,42 @@
             <text:p>Description</text:p>
           </table:table-cell>
         </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>course_title</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Master of Bábovka</text:p>
+          </table:table-cell>
+        </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>course_title</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Master of Bábovka</text:p>
+            <text:p>course_description</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Student se naučí připravit, upéct a naservírovat bábovku dle profesionálních pravidel</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell table:number-columns-repeated="2"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Final assessment type</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Mini-projekt</text:p>
           </table:table-cell>
         </table:table-row>
         <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>course_description</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Student se naučí připravit, upéct a naservírovat bábovku dle profesionálních pravidel</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell table:number-columns-repeated="2"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro4">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Final assessment type</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Mini-projekt + fotodokumentace výstupu</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro5">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Passing conditions</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>≥ 70 % celkem + ≥ 50 % kritická kritéria</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Badge reward</text:p>
           </table:table-cell>
@@ -160,7 +154,7 @@
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce2"/>
         <table:table-column table:style-name="co3" table:number-columns-repeated="2" table:default-cell-style-name="ce4"/>
         <table:table-column table:style-name="co3" table:number-columns-repeated="2" table:default-cell-style-name="ce2"/>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Module #</text:p>
           </table:table-cell>
@@ -180,7 +174,7 @@
             <text:p>Unlock Condition</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
             <text:p>1</text:p>
           </table:table-cell>
@@ -198,7 +192,7 @@
             <text:p>Always</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="float" office:value="2" calcext:value-type="float">
             <text:p>2</text:p>
           </table:table-cell>
@@ -216,7 +210,7 @@
             <text:p>Complete M1</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
             <text:p>3</text:p>
           </table:table-cell>
@@ -234,7 +228,7 @@
             <text:p>Complete M2</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="float" office:value="4" calcext:value-type="float">
             <text:p>4</text:p>
           </table:table-cell>
@@ -259,7 +253,7 @@
         <table:table-column table:style-name="co4" table:default-cell-style-name="ce2"/>
         <table:table-column table:style-name="co5" table:default-cell-style-name="ce2"/>
         <table:table-column table:style-name="co3" table:number-columns-repeated="2" table:default-cell-style-name="ce2"/>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Activity ID</text:p>
           </table:table-cell>
@@ -281,11 +275,9 @@
           <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
             <text:p>AI Mentor Hints?</text:p>
           </table:table-cell>
-          <table:table-cell table:style-name="ce1" office:value-type="string" calcext:value-type="string">
-            <text:p>Requires Portfolio?</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell table:style-name="ce1"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A1</text:p>
           </table:table-cell>
@@ -301,11 +293,12 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Krátká teorie + příklady</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>No</text:p>
           </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro4">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A2</text:p>
           </table:table-cell>
@@ -324,11 +317,12 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Vytvoř seznam ingrediencí</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Yes</text:p>
           </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A3</text:p>
           </table:table-cell>
@@ -348,13 +342,11 @@
             <text:p>3 otázky</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Auto</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>No</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+            <text:p>Yes</text:p>
+          </table:table-cell>
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A4</text:p>
           </table:table-cell>
@@ -371,13 +363,14 @@
             <text:p>Míchání těsta</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Video + vysvětlení</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
+            <text:p>vysvětlení</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>No</text:p>
           </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A5</text:p>
           </table:table-cell>
@@ -396,11 +389,9 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Yes</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>No</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A6</text:p>
           </table:table-cell>
@@ -417,16 +408,14 @@
             <text:p>Popiš těsto</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Text + foto těsta</text:p>
+            <text:p>Text</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>AI Evaluator</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Yes</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A7</text:p>
           </table:table-cell>
@@ -445,11 +434,12 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Pevná teplota &amp; čas</text:p>
           </table:table-cell>
-          <table:table-cell table:number-columns-repeated="2" office:value-type="string" calcext:value-type="string">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>No</text:p>
           </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A8</text:p>
           </table:table-cell>
@@ -466,16 +456,14 @@
             <text:p>Průběh pečení</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Foto každých 15 min</text:p>
+            <text:p>Popis</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>AI Evaluator</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Yes</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A9</text:p>
           </table:table-cell>
@@ -497,11 +485,9 @@
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Yes</text:p>
           </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>No</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
+          <table:table-cell/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A10</text:p>
           </table:table-cell>
@@ -521,11 +507,9 @@
             <text:p>3 otázky s analýzou</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Auto</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Yes</text:p>
           </table:table-cell>
+          <table:table-cell/>
         </table:table-row>
       </table:table>
       <table:table table:name="rubrics" table:style-name="ta1">
@@ -534,7 +518,7 @@
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce5"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce6"/>
         <table:table-column table:style-name="co3" table:default-cell-style-name="ce2"/>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell table:style-name="ce3" office:value-type="string" calcext:value-type="string">
             <text:p>Activity ID</text:p>
           </table:table-cell>
@@ -551,58 +535,58 @@
             <text:p>Description</text:p>
           </table:table-cell>
         </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A6</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Konzistence těsta</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>50%</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Y</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Bez hrudek</text:p>
+          </table:table-cell>
+        </table:table-row>
         <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A6</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Konzistence těsta</text:p>
+            <text:p>Pochopení postupu</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>50%</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>N</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Logická posloupnost kroků</text:p>
+          </table:table-cell>
+        </table:table-row>
+        <table:table-row table:style-name="ro3">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>A8</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>Rovnoměrnost pečení</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>70%</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Y</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Bez hrudek</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro4">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>A6</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Pochopení postupu</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>50%</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>N</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Logická posloupnost kroků</text:p>
-          </table:table-cell>
-        </table:table-row>
-        <table:table-row table:style-name="ro2">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>A8</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Rovnoměrnost pečení</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>70%</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>Y</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>Nespálené, ne syrové</text:p>
           </table:table-cell>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>A8</text:p>
           </table:table-cell>
@@ -630,11 +614,11 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.3">
   <office:meta>
     <meta:creation-date>2025-10-28T09:35:28.306444469</meta:creation-date>
-    <dc:date>2025-10-28T09:45:52.281210804</dc:date>
-    <meta:editing-duration>PT10M24S</meta:editing-duration>
-    <meta:editing-cycles>1</meta:editing-cycles>
+    <dc:date>2025-10-30T14:37:18.683524253</dc:date>
+    <meta:editing-duration>PT15M</meta:editing-duration>
+    <meta:editing-cycles>5</meta:editing-cycles>
     <meta:generator>LibreOffice/24.2.7.2$Linux_X86_64 LibreOffice_project/420$Build-2</meta:generator>
-    <meta:document-statistic meta:table-count="4" meta:cell-count="153" meta:object-count="0"/>
+    <meta:document-statistic meta:table-count="4" meta:cell-count="142" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
 </file>
@@ -645,22 +629,22 @@
     <config:config-item-set config:name="ooo:view-settings">
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
-      <config:config-item config:name="VisibleAreaWidth" config:type="int">9068</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">9506</config:config-item>
+      <config:config-item config:name="VisibleAreaWidth" config:type="int">22973</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">5747</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
           <config:config-item-map-named config:name="Tables">
             <config:config-item-map-entry config:name="activities">
               <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">18</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">13</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">243</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
               <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
@@ -669,15 +653,15 @@
               <config:config-item config:name="IgnoreBreakAfterMultilineField" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="course">
-              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">4</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">1</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">14</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">243</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
               <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
@@ -686,15 +670,15 @@
               <config:config-item config:name="IgnoreBreakAfterMultilineField" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="modules">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">13</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">5</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">3</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
               <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">243</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
               <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
@@ -711,7 +695,7 @@
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionBottom" config:type="int">0</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-              <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+              <config:config-item config:name="ZoomValue" config:type="int">243</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
               <config:config-item config:name="ShowGrid" config:type="boolean">true</config:config-item>
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
@@ -720,10 +704,10 @@
               <config:config-item config:name="IgnoreBreakAfterMultilineField" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
           </config:config-item-map-named>
-          <config:config-item config:name="ActiveTable" config:type="string">activities</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">2437</config:config-item>
+          <config:config-item config:name="ActiveTable" config:type="string">rubrics</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">2489</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
-          <config:config-item config:name="ZoomValue" config:type="int">100</config:config-item>
+          <config:config-item config:name="ZoomValue" config:type="int">243</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
           <config:config-item config:name="ShowPageBreakPreview" config:type="boolean">false</config:config-item>
           <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
@@ -780,9 +764,9 @@
       <config:config-item config:name="IsSnapToRaster" config:type="boolean">false</config:config-item>
       <config:config-item config:name="LinkUpdateMode" config:type="short">3</config:config-item>
       <config:config-item config:name="LoadReadonly" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterName" config:type="string"/>
+      <config:config-item config:name="PrinterName" config:type="string">HP_DeskJet_3700_series_A8E35D</config:config-item>
       <config:config-item config:name="PrinterPaperFromSetup" config:type="boolean">false</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary"/>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">7wH+/0hQX0Rlc2tKZXRfMzcwMF9zZXJpZXNfQThFMzVEAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAQ1VQUzpIUF9EZXNrSmV0XzM3MDBfc2VyaWVzX0E4RQAWAAMArgAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9SFBfRGVza0pldF8zNzAwX3Nlcmllc19BOEUzNUQKb3JpZW50YXRpb249UG9ydHJhaXQKY29waWVzPTEKY29sbGF0ZT1mYWxzZQptYXJnaW5hZGp1c3RtZW50PTAsMCwnMCwwCmNvbG9yZGVwdGg9MjQKY29sb3JkZXZpY2U9MApQUERDb250ZXh0RGF0YQpQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUTAER1cGxleE1vZGU6OlVua25vd24MAFBSSU5URVJfTkFNRR0ASFBfRGVza0pldF8zNzAwX3Nlcmllc19BOEUzNUQLAERSSVZFUl9OQU1FIgBDVVBTOkhQX0Rlc2tKZXRfMzcwMF9zZXJpZXNfQThFMzVE</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1270</config:config-item>
       <config:config-item config:name="RasterResolutionY" config:type="int">1270</config:config-item>
@@ -795,6 +779,7 @@
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowPageBreaks" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowZeroValues" config:type="boolean">true</config:config-item>
+      <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="UpdateFromTemplate" config:type="boolean">true</config:config-item>
       <config:config-item-map-named config:name="ScriptConfiguration">
         <config:config-item-map-entry config:name="course">
@@ -831,7 +816,7 @@
     </style:default-style>
     <style:default-style style:family="graphic">
       <style:graphic-properties svg:stroke-color="#3465a4" draw:fill-color="#729fcf" fo:wrap-option="no-wrap" draw:shadow-offset-x="0.1181in" draw:shadow-offset-y="0.1181in" style:writing-mode="page"/>
-      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" style:writing-mode="page" style:font-independent-line-spacing="false">
+      <style:paragraph-properties style:text-autospace="ideograph-alpha" style:punctuation-wrap="simple" style:line-break="strict" loext:tab-stop-distance="0in" style:writing-mode="page" style:font-independent-line-spacing="false">
         <style:tab-stops/>
       </style:paragraph-properties>
       <style:text-properties style:use-window-font-color="true" loext:opacity="0%" style:font-name="Liberation Serif" fo:font-size="12pt" fo:language="en" fo:country="US" style:letter-kerning="true" style:font-name-asian="DejaVu Sans" style:font-size-asian="12pt" style:language-asian="zh" style:country-asian="CN" style:font-name-complex="DejaVu Sans" style:font-size-complex="12pt" style:language-complex="hi" style:country-complex="IN"/>
@@ -990,9 +975,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2025-10-28">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2025-10-30">00/00/0000</text:date>
             , 
-            <text:time>00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="14:32:41.683740144">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>